<commit_message>
calculated how many 5dof configurations left
</commit_message>
<xml_diff>
--- a/general/לעשות.xlsx
+++ b/general/לעשות.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t xml:space="preserve">מס'</t>
   </si>
@@ -352,7 +352,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -443,7 +443,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="1" sqref="C11:C12 C16"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -507,7 +507,9 @@
       <c r="B3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="D3" s="11" t="s">
         <v>12</v>
       </c>
@@ -539,7 +541,9 @@
       <c r="B5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="D5" s="11"/>
       <c r="E5" s="13"/>
       <c r="F5" s="14"/>

</xml_diff>

<commit_message>
create json file with all the concepts, all the configurations of each concept, and if the configuration is simulated what its indices
</commit_message>
<xml_diff>
--- a/general/לעשות.xlsx
+++ b/general/לעשות.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t xml:space="preserve">מס'</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">קונספטים שבדקתי את הרוב - לסיים </t>
+  </si>
+  <si>
+    <t xml:space="preserve">running</t>
   </si>
   <si>
     <t xml:space="preserve">גודל קונספט</t>
@@ -443,7 +446,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -526,9 +529,11 @@
       <c r="B4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="D4" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="14"/>
@@ -539,7 +544,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>8</v>
@@ -555,7 +560,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>8</v>
@@ -570,7 +575,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="11"/>
@@ -583,7 +588,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" s="12" t="n">
         <v>1</v>
@@ -598,7 +603,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="11"/>
@@ -611,7 +616,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="11"/>
@@ -624,7 +629,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>8</v>
@@ -639,7 +644,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>8</v>

</xml_diff>